<commit_message>
Update Excel file with new submissions
</commit_message>
<xml_diff>
--- a/data/submissions.xlsx
+++ b/data/submissions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -709,6 +709,98 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ggs</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hhshs</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hhsh</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hhshs</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>